<commit_message>
Excel para mostrar (imputa)
Excel para mostrar
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/Old/VEN_income_imputation_old.xlsx
+++ b/data_management/management/4. income imputation/output/Old/VEN_income_imputation_old.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB469948\OneDrive - WBG\LAC\Venezuela\Income Imputation\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb563583\GitHub\VEN\data_management\management\4. income imputation\output\Old\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_7FBAEC184D1CE943FC229CAA0C7A62580C73E2CB" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{149068E2-86D0-489F-AA9A-22D441184F00}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317A155E-0C71-42BF-989D-CDE2295EADEF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="income in official estimates" sheetId="10" r:id="rId1"/>
@@ -42264,36 +42264,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="J12:K12"/>
     <mergeCell ref="L52:M52"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="D62:E62"/>
@@ -42306,6 +42276,36 @@
     <mergeCell ref="F52:G52"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="J52:K52"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="J42:K42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -42561,8 +42561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45297,7 +45297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -46924,18 +46924,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47162,6 +47162,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBC7312B-146D-4237-A5EF-98BD773A41DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12907964-CBB5-465B-8DF5-7CBD485C36A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -47174,14 +47182,6 @@
     <ds:schemaRef ds:uri="72d74521-8c27-4702-99f8-167624e069b6"/>
     <ds:schemaRef ds:uri="69ca14ff-5d6d-4eb8-91d9-74d4bb4de445"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBC7312B-146D-4237-A5EF-98BD773A41DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>